<commit_message>
fixed bugs and did a few runs
</commit_message>
<xml_diff>
--- a/Equivalent_Widths/norm_RVcorr_LHS72.txt_EWs.xlsx
+++ b/Equivalent_Widths/norm_RVcorr_LHS72.txt_EWs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapta\Desktop\Atmospheric_Studies_VLMS\Abundance_Estimation_EW\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapta\Desktop\Atmospheric_Studies_VLMS\Equivalent_Widths\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37F47268-FE3B-4682-BCF1-9169463EE6BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BCDC2FC-2E78-4F32-8D03-22BDD1913B49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="168" windowWidth="17280" windowHeight="12072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="15">
   <si>
     <t>Absorption_Lines_(A)</t>
   </si>
@@ -47,6 +47,15 @@
   </si>
   <si>
     <t>Ca I</t>
+  </si>
+  <si>
+    <t>Ti I</t>
+  </si>
+  <si>
+    <t>Fe I</t>
+  </si>
+  <si>
+    <t>Na I</t>
   </si>
   <si>
     <t>Lorentzian</t>
@@ -62,8 +71,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -79,12 +96,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -93,7 +125,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -434,22 +466,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H10"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="A1:H1"/>
+      <selection sqref="A1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="8.21875" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="10.109375" customWidth="1"/>
-    <col min="6" max="6" width="10.44140625" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="8" max="8" width="11.88671875" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
@@ -495,7 +520,7 @@
         <v>6465.17</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G2">
         <v>0.33926832102559179</v>
@@ -521,7 +546,7 @@
         <v>6474.4</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G3">
         <v>0.18681501847893281</v>
@@ -547,7 +572,7 @@
         <v>6497.7</v>
       </c>
       <c r="F4" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="G4">
         <v>0.28934140436837769</v>
@@ -573,7 +598,7 @@
         <v>6502.8</v>
       </c>
       <c r="F5" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="G5">
         <v>0.14385603540007019</v>
@@ -584,136 +609,759 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>6574.561686</v>
+        <v>6556.0097489999998</v>
       </c>
       <c r="B6">
-        <v>6574.5950000000003</v>
+        <v>6556.0335999999998</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D6">
-        <v>6573.7</v>
+        <v>6555.4</v>
       </c>
       <c r="E6">
-        <v>6575.4</v>
+        <v>6556.7</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="G6">
-        <v>0.1393475869694169</v>
+        <v>4.7337000242964389E-2</v>
       </c>
       <c r="H6">
-        <v>3.7521879204125571E-3</v>
+        <v>9.5902186962364415E-4</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>6719.5097159999996</v>
+        <v>6557.8512300000002</v>
       </c>
       <c r="B7">
-        <v>6719.5360000000001</v>
+        <v>6557.8729000000003</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D7">
-        <v>6718.3</v>
+        <v>6557</v>
       </c>
       <c r="E7">
-        <v>6720.8</v>
+        <v>6558.3</v>
       </c>
       <c r="F7" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G7">
-        <v>0.2157192683602569</v>
+        <v>5.5819756314121678E-2</v>
       </c>
       <c r="H7">
-        <v>8.5341303409829754E-3</v>
+        <v>1.142432496380918E-3</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>7150.1027260000001</v>
+        <v>6574.561686</v>
       </c>
       <c r="B8">
-        <v>7150</v>
+        <v>6574.5950000000003</v>
       </c>
       <c r="C8" t="s">
         <v>8</v>
       </c>
       <c r="D8">
-        <v>7149</v>
+        <v>6573.7</v>
       </c>
       <c r="E8">
-        <v>7151.7</v>
+        <v>6575.4</v>
       </c>
       <c r="F8" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="G8">
-        <v>0.29791095479552337</v>
+        <v>0.1393475869694169</v>
       </c>
       <c r="H8">
-        <v>1.2731216217229731E-2</v>
+        <v>3.7521879204125571E-3</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>7204.1521389999998</v>
+        <v>6594.7200220000004</v>
       </c>
       <c r="B9">
-        <v>7204</v>
+        <v>6594.7331000000004</v>
       </c>
       <c r="C9" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D9">
-        <v>7203</v>
+        <v>6593</v>
       </c>
       <c r="E9">
-        <v>7206.4</v>
+        <v>6597</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="G9">
-        <v>0.22473521424353751</v>
+        <v>8.693036638182379E-2</v>
       </c>
       <c r="H9">
-        <v>1.196891326161377E-2</v>
+        <v>5.5071592621077003E-3</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10">
+        <v>6595.6603519999999</v>
+      </c>
+      <c r="B10">
+        <v>6595.6904000000004</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>6593</v>
+      </c>
+      <c r="E10">
+        <v>6597</v>
+      </c>
+      <c r="F10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>3.4255819089064603E-2</v>
+      </c>
+      <c r="H10">
+        <v>2.1488637223311411E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>6600.8909409999997</v>
+      </c>
+      <c r="B11">
+        <v>6600.9285</v>
+      </c>
+      <c r="C11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <v>6600.2</v>
+      </c>
+      <c r="E11">
+        <v>6601.8</v>
+      </c>
+      <c r="F11" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11">
+        <v>4.305878699005225E-2</v>
+      </c>
+      <c r="H11">
+        <v>1.041077553156569E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>6665.2448089999998</v>
+      </c>
+      <c r="B12">
+        <v>6665.2807000000003</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12">
+        <v>6664.41</v>
+      </c>
+      <c r="E12">
+        <v>6665.9</v>
+      </c>
+      <c r="F12" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12">
+        <v>3.6904155890789339E-2</v>
+      </c>
+      <c r="H12">
+        <v>8.5828610465792446E-4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>6679.8199320000003</v>
+      </c>
+      <c r="B13">
+        <v>6679.8285999999998</v>
+      </c>
+      <c r="C13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13">
+        <v>6678.3</v>
+      </c>
+      <c r="E13">
+        <v>6680.6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13">
+        <v>0.1097471746655698</v>
+      </c>
+      <c r="H13">
+        <v>3.8760421214573629E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>6719.5097159999996</v>
+      </c>
+      <c r="B14">
+        <v>6719.5360000000001</v>
+      </c>
+      <c r="C14" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14">
+        <v>6718.3</v>
+      </c>
+      <c r="E14">
+        <v>6720.8</v>
+      </c>
+      <c r="F14" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14">
+        <v>0.2157192683602569</v>
+      </c>
+      <c r="H14">
+        <v>8.5341303409829754E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>7150.1027260000001</v>
+      </c>
+      <c r="B15">
+        <v>7150</v>
+      </c>
+      <c r="C15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15">
+        <v>7149</v>
+      </c>
+      <c r="E15">
+        <v>7151.7</v>
+      </c>
+      <c r="F15" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15">
+        <v>0.29791095479552337</v>
+      </c>
+      <c r="H15">
+        <v>1.2731216217229731E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>7204.1521389999998</v>
+      </c>
+      <c r="B16">
+        <v>7204</v>
+      </c>
+      <c r="C16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16">
+        <v>7203</v>
+      </c>
+      <c r="E16">
+        <v>7206.4</v>
+      </c>
+      <c r="F16" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16">
+        <v>0.22473521424353751</v>
+      </c>
+      <c r="H16">
+        <v>1.196891326161377E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>7211.4005200000001</v>
+      </c>
+      <c r="B17">
+        <v>7211.4228000000003</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17">
+        <v>7210.75</v>
+      </c>
+      <c r="E17">
+        <v>7212.25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>14</v>
+      </c>
+      <c r="G17">
+        <v>0.1075179112187007</v>
+      </c>
+      <c r="H17">
+        <v>2.5403581709072189E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>7246.8196360000002</v>
+      </c>
+      <c r="B18">
+        <v>7246.8509999999997</v>
+      </c>
+      <c r="C18" t="s">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>7245.66</v>
+      </c>
+      <c r="E18">
+        <v>7247.69</v>
+      </c>
+      <c r="F18" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18">
+        <v>8.0573172390381975E-2</v>
+      </c>
+      <c r="H18">
+        <v>2.7810916512337079E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7253.6762129999997</v>
+      </c>
+      <c r="B19">
+        <v>7253.7078000000001</v>
+      </c>
+      <c r="C19" t="s">
+        <v>9</v>
+      </c>
+      <c r="D19">
+        <v>7252.17</v>
+      </c>
+      <c r="E19">
+        <v>7255</v>
+      </c>
+      <c r="F19" t="s">
+        <v>14</v>
+      </c>
+      <c r="G19">
+        <v>8.2045143321283431E-2</v>
+      </c>
+      <c r="H19">
+        <v>4.0045826755135518E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20">
         <v>7328.1386339999999</v>
       </c>
-      <c r="B10">
+      <c r="B20">
         <v>7328</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C20" t="s">
         <v>8</v>
       </c>
-      <c r="D10">
+      <c r="D20">
         <v>7327</v>
       </c>
-      <c r="E10">
+      <c r="E20">
         <v>7329.5</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F20" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20">
+        <v>0.25125449335676192</v>
+      </c>
+      <c r="H20">
+        <v>1.016079138694332E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>7346.6905720000004</v>
+      </c>
+      <c r="B21">
+        <v>7346.7186000000002</v>
+      </c>
+      <c r="C21" t="s">
         <v>9</v>
       </c>
-      <c r="G10">
-        <v>0.25125449335676192</v>
-      </c>
-      <c r="H10">
-        <v>1.016079138694332E-2</v>
+      <c r="D21">
+        <v>7346.13</v>
+      </c>
+      <c r="E21">
+        <v>7347.64</v>
+      </c>
+      <c r="F21" t="s">
+        <v>14</v>
+      </c>
+      <c r="G21">
+        <v>6.7548806206560424E-2</v>
+      </c>
+      <c r="H21">
+        <v>1.62198605623213E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>7359.7376569999997</v>
+      </c>
+      <c r="B22">
+        <v>7359.7538000000004</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>7358.66</v>
+      </c>
+      <c r="E22">
+        <v>7360.35</v>
+      </c>
+      <c r="F22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G22">
+        <v>5.8305622545934702E-2</v>
+      </c>
+      <c r="H22">
+        <v>1.6318578662742891E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>7366.1240690000004</v>
+      </c>
+      <c r="B23">
+        <v>7366.1297999999997</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23">
+        <v>7365.3</v>
+      </c>
+      <c r="E23">
+        <v>7367</v>
+      </c>
+      <c r="F23" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23">
+        <v>5.0460622051176428E-2</v>
+      </c>
+      <c r="H23">
+        <v>1.337972819023355E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>7666.3833530000002</v>
+      </c>
+      <c r="B24">
+        <v>7666.4029</v>
+      </c>
+      <c r="C24" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>7664</v>
+      </c>
+      <c r="E24">
+        <v>7669.4</v>
+      </c>
+      <c r="F24" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24">
+        <v>0.66331373952994088</v>
+      </c>
+      <c r="H24">
+        <v>5.7795603623618408E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>8185.5045620000001</v>
+      </c>
+      <c r="B25">
+        <v>8185.5052999999998</v>
+      </c>
+      <c r="C25" t="s">
+        <v>11</v>
+      </c>
+      <c r="D25">
+        <v>8184.05</v>
+      </c>
+      <c r="E25">
+        <v>8187</v>
+      </c>
+      <c r="F25" t="s">
+        <v>13</v>
+      </c>
+      <c r="G25">
+        <v>0.1978833885997712</v>
+      </c>
+      <c r="H25">
+        <v>9.5666415953601213E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>8437.2584640000005</v>
+      </c>
+      <c r="B26">
+        <v>8437.2720000000008</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26">
+        <v>8434</v>
+      </c>
+      <c r="E26">
+        <v>8440</v>
+      </c>
+      <c r="F26" t="s">
+        <v>13</v>
+      </c>
+      <c r="G26">
+        <v>0.24010963024917209</v>
+      </c>
+      <c r="H26">
+        <v>2.0731458616329249E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>8437.9637120000007</v>
+      </c>
+      <c r="B27">
+        <v>8437.9699999999993</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27">
+        <v>8434</v>
+      </c>
+      <c r="E27">
+        <v>8440</v>
+      </c>
+      <c r="F27" t="s">
+        <v>13</v>
+      </c>
+      <c r="G27">
+        <v>0.2083796508442356</v>
+      </c>
+      <c r="H27">
+        <v>1.799184024180682E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>8470.7381480000004</v>
+      </c>
+      <c r="B28">
+        <v>8470.7329000000009</v>
+      </c>
+      <c r="C28" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28">
+        <v>8468.35</v>
+      </c>
+      <c r="E28">
+        <v>8472</v>
+      </c>
+      <c r="F28" t="s">
+        <v>13</v>
+      </c>
+      <c r="G28">
+        <v>0.14203046266359909</v>
+      </c>
+      <c r="H28">
+        <v>7.6037768549504616E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>8516.4029480000008</v>
+      </c>
+      <c r="B29">
+        <v>8516.4105999999992</v>
+      </c>
+      <c r="C29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>8515</v>
+      </c>
+      <c r="E29">
+        <v>8518.5</v>
+      </c>
+      <c r="F29" t="s">
+        <v>13</v>
+      </c>
+      <c r="G29">
+        <v>0.1048751039438189</v>
+      </c>
+      <c r="H29">
+        <v>5.7749971204432617E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>8677.1211039999998</v>
+      </c>
+      <c r="B30">
+        <v>8677.1283999999996</v>
+      </c>
+      <c r="C30" t="s">
+        <v>10</v>
+      </c>
+      <c r="D30">
+        <v>8675</v>
+      </c>
+      <c r="E30">
+        <v>8679</v>
+      </c>
+      <c r="F30" t="s">
+        <v>13</v>
+      </c>
+      <c r="G30">
+        <v>7.0197456707723815E-2</v>
+      </c>
+      <c r="H30">
+        <v>4.0914960906903684E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>8677.7479910000002</v>
+      </c>
+      <c r="B31">
+        <v>8677.7549999999992</v>
+      </c>
+      <c r="C31" t="s">
+        <v>9</v>
+      </c>
+      <c r="D31">
+        <v>8675</v>
+      </c>
+      <c r="E31">
+        <v>8679</v>
+      </c>
+      <c r="F31" t="s">
+        <v>13</v>
+      </c>
+      <c r="G31">
+        <v>8.9141027947865992E-2</v>
+      </c>
+      <c r="H31">
+        <v>5.1956322133916363E-3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>8685.3685860000005</v>
+      </c>
+      <c r="B32">
+        <v>8685.3680000000004</v>
+      </c>
+      <c r="C32" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32">
+        <v>8684</v>
+      </c>
+      <c r="E32">
+        <v>8687</v>
+      </c>
+      <c r="F32" t="s">
+        <v>14</v>
+      </c>
+      <c r="G32">
+        <v>5.6742799803900949E-2</v>
+      </c>
+      <c r="H32">
+        <v>2.4715102308592641E-3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>8690.9909779999998</v>
+      </c>
+      <c r="B33">
+        <v>8691.0097000000005</v>
+      </c>
+      <c r="C33" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>8688</v>
+      </c>
+      <c r="E33">
+        <v>8694</v>
+      </c>
+      <c r="F33" t="s">
+        <v>12</v>
+      </c>
+      <c r="G33">
+        <v>0.34612480026483378</v>
+      </c>
+      <c r="H33">
+        <v>3.0040897440273519E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>8826.6336539999993</v>
+      </c>
+      <c r="B34">
+        <v>8826.6425999999992</v>
+      </c>
+      <c r="C34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D34">
+        <v>8824</v>
+      </c>
+      <c r="E34">
+        <v>8830</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34">
+        <v>0.24109869830169151</v>
+      </c>
+      <c r="H34">
+        <v>2.06236332523594E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>